<commit_message>
small tweak to p.c
</commit_message>
<xml_diff>
--- a/data/gb/parameter_ranges.xlsx
+++ b/data/gb/parameter_ranges.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="0" windowWidth="18820" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="-12520" yWindow="0" windowWidth="12500" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1297,13 +1297,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="14">
-        <v>0.14899999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="D21" s="14">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E21" s="14">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>46</v>
@@ -1320,13 +1320,13 @@
         <v>9</v>
       </c>
       <c r="C22" s="16">
-        <v>0.14899999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="D22" s="16">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E22" s="16">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>46</v>
@@ -1341,13 +1341,13 @@
         <v>10</v>
       </c>
       <c r="C23" s="16">
-        <v>0.27300000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="D23" s="16">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="16">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="F23" s="15" t="s">
         <v>46</v>
@@ -1362,13 +1362,13 @@
         <v>11</v>
       </c>
       <c r="C24" s="16">
-        <v>0.23300000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D24" s="16">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E24" s="16">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>46</v>
@@ -1383,13 +1383,13 @@
         <v>12</v>
       </c>
       <c r="C25" s="16">
-        <v>0.23300000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D25" s="16">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E25" s="16">
-        <v>0.25</v>
+        <v>0.26</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>46</v>
@@ -1404,13 +1404,13 @@
         <v>13</v>
       </c>
       <c r="C26" s="18">
-        <v>0.27300000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="D26" s="18">
-        <v>0.22</v>
+        <v>0.25</v>
       </c>
       <c r="E26" s="18">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>46</v>

</xml_diff>